<commit_message>
Fixing Agenda Mobile and portal
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_Digisales/SCD0338-008 - View agenda pada Portal.xlsx
+++ b/Lib_Repo_Excel/FileExcel_Digisales/SCD0338-008 - View agenda pada Portal.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20584CD6-AF7F-428C-ABEC-2D4C2F34B422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B6C148-2865-44F5-96A0-85D97831DA79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -549,7 +549,7 @@
   <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="66" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,7 +680,7 @@
         <v>33</v>
       </c>
       <c r="Q2" s="1" t="str">
-        <f ca="1">TEXT(TODAY(),"mmmm")</f>
+        <f ca="1">TEXT(TODAY()-30,"mmmm")</f>
         <v>October</v>
       </c>
     </row>
@@ -730,7 +730,7 @@
         <v>25</v>
       </c>
       <c r="Q3" s="1" t="str">
-        <f ca="1">TEXT(TODAY(),"mmmm")</f>
+        <f ca="1">TEXT(TODAY()-30,"mmmm")</f>
         <v>October</v>
       </c>
     </row>

</xml_diff>